<commit_message>
feat(monsters): added more monsters to the excel file
</commit_message>
<xml_diff>
--- a/monsters.xlsx
+++ b/monsters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eterspire - Fantasy MMORPG_43.2_APKPure\Monster Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eterspire Wiki Work\Monster Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6535DA1B-E1B7-41BA-AF00-8152928F5AC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF67EE53-273E-4C73-B38B-C2BED11CE51B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9228" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="145">
   <si>
     <t>name</t>
   </si>
@@ -321,6 +321,141 @@
   </si>
   <si>
     <t>Poison</t>
+  </si>
+  <si>
+    <t>Pyramid Snake</t>
+  </si>
+  <si>
+    <t>Am-Rawash's Tomb (Southeast)</t>
+  </si>
+  <si>
+    <t>54 - 69</t>
+  </si>
+  <si>
+    <t>Cursed Mummy</t>
+  </si>
+  <si>
+    <t>Possessed Mummy</t>
+  </si>
+  <si>
+    <t>Am-Rawash's Sepulcher</t>
+  </si>
+  <si>
+    <t>Moored Soul</t>
+  </si>
+  <si>
+    <t>Ghost Speck</t>
+  </si>
+  <si>
+    <t>Dark Moor</t>
+  </si>
+  <si>
+    <t>Stun</t>
+  </si>
+  <si>
+    <t>Phantasm</t>
+  </si>
+  <si>
+    <t>Pyramid Graveyard</t>
+  </si>
+  <si>
+    <t>Quartz Beetle</t>
+  </si>
+  <si>
+    <t>143 - 167</t>
+  </si>
+  <si>
+    <t>Stalking Demon</t>
+  </si>
+  <si>
+    <t>Twilight Dunes</t>
+  </si>
+  <si>
+    <t>Slow</t>
+  </si>
+  <si>
+    <t>Roaming Deer</t>
+  </si>
+  <si>
+    <t>Spire Valley</t>
+  </si>
+  <si>
+    <t>Cartesian Dungeon</t>
+  </si>
+  <si>
+    <t>Island Scorpion</t>
+  </si>
+  <si>
+    <t>Not-So-Squishy Crabby</t>
+  </si>
+  <si>
+    <t>Poison, Blind</t>
+  </si>
+  <si>
+    <t>Crusher Demon</t>
+  </si>
+  <si>
+    <t>Cartesian Beast</t>
+  </si>
+  <si>
+    <t>Cartesian Ghoul</t>
+  </si>
+  <si>
+    <t>154 - 171</t>
+  </si>
+  <si>
+    <t>Vestadian Bridge</t>
+  </si>
+  <si>
+    <t>Giant Frosty Speck</t>
+  </si>
+  <si>
+    <t>61-71</t>
+  </si>
+  <si>
+    <t>Highland Spider</t>
+  </si>
+  <si>
+    <t>61-72</t>
+  </si>
+  <si>
+    <t>Frosty Speck</t>
+  </si>
+  <si>
+    <t>Snowy Hills</t>
+  </si>
+  <si>
+    <t>Pomel</t>
+  </si>
+  <si>
+    <t>Black Wolf</t>
+  </si>
+  <si>
+    <t>128 - 154</t>
+  </si>
+  <si>
+    <t>Snow Burrower</t>
+  </si>
+  <si>
+    <t>Frost Crevasse</t>
+  </si>
+  <si>
+    <t>135 - 162</t>
+  </si>
+  <si>
+    <t>Mountain Wolf</t>
+  </si>
+  <si>
+    <t>Greater Emeraldion</t>
+  </si>
+  <si>
+    <t>Green Temple II</t>
+  </si>
+  <si>
+    <t>Emeraldion Guardian</t>
+  </si>
+  <si>
+    <t>Green Temple III</t>
   </si>
 </sst>
 </file>
@@ -341,7 +476,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -351,6 +486,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -367,9 +508,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,20 +826,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F537407C-ED86-44CA-B9EC-6F634CBFD2ED}">
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
     <col min="2" max="2" width="44.33203125" customWidth="1"/>
     <col min="3" max="3" width="4.88671875" customWidth="1"/>
     <col min="4" max="4" width="28.109375" customWidth="1"/>
     <col min="5" max="5" width="7.5546875" customWidth="1"/>
-    <col min="6" max="6" width="7.88671875" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" customWidth="1"/>
     <col min="7" max="7" width="4.33203125" customWidth="1"/>
     <col min="8" max="8" width="53.6640625" customWidth="1"/>
     <col min="9" max="9" width="7.109375" customWidth="1"/>
@@ -2151,55 +2293,604 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>9</v>
-      </c>
-      <c r="C51">
-        <v>0</v>
-      </c>
-      <c r="D51" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" t="s">
-        <v>10</v>
-      </c>
-      <c r="F51" t="s">
-        <v>72</v>
-      </c>
-      <c r="G51">
-        <v>0</v>
-      </c>
-      <c r="H51" t="s">
-        <v>52</v>
-      </c>
-      <c r="I51">
-        <v>0</v>
-      </c>
+      <c r="B51" s="2"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>9</v>
+        <v>100</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D52" t="s">
-        <v>9</v>
+        <v>101</v>
       </c>
       <c r="E52" t="s">
         <v>10</v>
       </c>
       <c r="F52" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="G52">
-        <v>0</v>
+        <v>296</v>
       </c>
       <c r="H52" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>134</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C53">
+        <v>60</v>
+      </c>
+      <c r="D53" t="s">
+        <v>133</v>
+      </c>
+      <c r="E53" t="s">
+        <v>109</v>
+      </c>
+      <c r="F53" t="s">
+        <v>102</v>
+      </c>
+      <c r="G53">
+        <v>296</v>
+      </c>
+      <c r="H53" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>141</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C54">
+        <v>61</v>
+      </c>
+      <c r="D54" t="s">
+        <v>142</v>
+      </c>
+      <c r="E54" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" t="s">
+        <v>129</v>
+      </c>
+      <c r="G54">
+        <v>300</v>
+      </c>
+      <c r="H54" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>132</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C55">
+        <v>61</v>
+      </c>
+      <c r="D55" t="s">
+        <v>133</v>
+      </c>
+      <c r="E55" t="s">
+        <v>116</v>
+      </c>
+      <c r="F55" t="s">
+        <v>129</v>
+      </c>
+      <c r="G55">
+        <v>300</v>
+      </c>
+      <c r="H55" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>128</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C56">
+        <v>61</v>
+      </c>
+      <c r="D56" t="s">
+        <v>127</v>
+      </c>
+      <c r="E56" t="s">
+        <v>116</v>
+      </c>
+      <c r="F56" t="s">
+        <v>129</v>
+      </c>
+      <c r="G56">
+        <v>300</v>
+      </c>
+      <c r="H56" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>130</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C57">
+        <v>62</v>
+      </c>
+      <c r="D57" t="s">
+        <v>127</v>
+      </c>
+      <c r="E57" t="s">
+        <v>99</v>
+      </c>
+      <c r="F57" t="s">
+        <v>131</v>
+      </c>
+      <c r="G57">
+        <v>305</v>
+      </c>
+      <c r="H57" t="s">
         <v>52</v>
       </c>
-      <c r="I52">
-        <v>0</v>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>103</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C58">
+        <v>62</v>
+      </c>
+      <c r="D58" t="s">
+        <v>101</v>
+      </c>
+      <c r="E58" t="s">
+        <v>10</v>
+      </c>
+      <c r="F58" t="s">
+        <v>131</v>
+      </c>
+      <c r="G58">
+        <v>305</v>
+      </c>
+      <c r="H58" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>104</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C59">
+        <v>63</v>
+      </c>
+      <c r="D59" t="s">
+        <v>105</v>
+      </c>
+      <c r="E59" t="s">
+        <v>10</v>
+      </c>
+      <c r="F59" t="s">
+        <v>136</v>
+      </c>
+      <c r="G59">
+        <v>309</v>
+      </c>
+      <c r="H59" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>143</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C60">
+        <v>63</v>
+      </c>
+      <c r="D60" t="s">
+        <v>144</v>
+      </c>
+      <c r="E60" t="s">
+        <v>10</v>
+      </c>
+      <c r="F60" t="s">
+        <v>136</v>
+      </c>
+      <c r="G60">
+        <v>309</v>
+      </c>
+      <c r="H60" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>135</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C61">
+        <v>63</v>
+      </c>
+      <c r="D61" t="s">
+        <v>127</v>
+      </c>
+      <c r="E61" t="s">
+        <v>10</v>
+      </c>
+      <c r="F61" t="s">
+        <v>136</v>
+      </c>
+      <c r="G61">
+        <v>309</v>
+      </c>
+      <c r="H61" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>121</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C62">
+        <v>63</v>
+      </c>
+      <c r="D62" t="s">
+        <v>118</v>
+      </c>
+      <c r="E62" t="s">
+        <v>109</v>
+      </c>
+      <c r="F62" t="s">
+        <v>136</v>
+      </c>
+      <c r="G62">
+        <v>309</v>
+      </c>
+      <c r="H62" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>120</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C63">
+        <v>64</v>
+      </c>
+      <c r="D63" t="s">
+        <v>118</v>
+      </c>
+      <c r="E63" t="s">
+        <v>122</v>
+      </c>
+      <c r="F63" t="s">
+        <v>136</v>
+      </c>
+      <c r="G63">
+        <v>314</v>
+      </c>
+      <c r="H63" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>107</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C64">
+        <v>64</v>
+      </c>
+      <c r="D64" t="s">
+        <v>108</v>
+      </c>
+      <c r="E64" t="s">
+        <v>109</v>
+      </c>
+      <c r="F64" t="s">
+        <v>136</v>
+      </c>
+      <c r="G64">
+        <v>309</v>
+      </c>
+      <c r="H64" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>140</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C65">
+        <v>64</v>
+      </c>
+      <c r="D65" t="s">
+        <v>138</v>
+      </c>
+      <c r="E65" t="s">
+        <v>10</v>
+      </c>
+      <c r="F65" t="s">
+        <v>136</v>
+      </c>
+      <c r="G65">
+        <v>309</v>
+      </c>
+      <c r="H65" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>137</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C66">
+        <v>65</v>
+      </c>
+      <c r="D66" t="s">
+        <v>138</v>
+      </c>
+      <c r="E66" t="s">
+        <v>10</v>
+      </c>
+      <c r="F66" t="s">
+        <v>139</v>
+      </c>
+      <c r="G66">
+        <v>318</v>
+      </c>
+      <c r="H66" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>106</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C67">
+        <v>65</v>
+      </c>
+      <c r="D67" t="s">
+        <v>108</v>
+      </c>
+      <c r="E67" t="s">
+        <v>99</v>
+      </c>
+      <c r="F67" t="s">
+        <v>139</v>
+      </c>
+      <c r="G67">
+        <v>318</v>
+      </c>
+      <c r="H67" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>110</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C68">
+        <v>66</v>
+      </c>
+      <c r="D68" t="s">
+        <v>111</v>
+      </c>
+      <c r="E68" t="s">
+        <v>99</v>
+      </c>
+      <c r="F68" t="s">
+        <v>139</v>
+      </c>
+      <c r="G68">
+        <v>323</v>
+      </c>
+      <c r="H68" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>124</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C69">
+        <v>67</v>
+      </c>
+      <c r="D69" t="s">
+        <v>119</v>
+      </c>
+      <c r="E69" t="s">
+        <v>10</v>
+      </c>
+      <c r="F69" t="s">
+        <v>126</v>
+      </c>
+      <c r="G69">
+        <v>327</v>
+      </c>
+      <c r="H69" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>112</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C70">
+        <v>68</v>
+      </c>
+      <c r="D70" t="s">
+        <v>111</v>
+      </c>
+      <c r="E70" t="s">
+        <v>10</v>
+      </c>
+      <c r="F70" t="s">
+        <v>113</v>
+      </c>
+      <c r="G70">
+        <v>332</v>
+      </c>
+      <c r="H70" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>117</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C71">
+        <v>69</v>
+      </c>
+      <c r="D71" t="s">
+        <v>115</v>
+      </c>
+      <c r="E71" t="s">
+        <v>14</v>
+      </c>
+      <c r="F71" t="s">
+        <v>113</v>
+      </c>
+      <c r="G71">
+        <v>336</v>
+      </c>
+      <c r="H71" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>123</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C72">
+        <v>69</v>
+      </c>
+      <c r="D72" t="s">
+        <v>119</v>
+      </c>
+      <c r="E72" t="s">
+        <v>109</v>
+      </c>
+      <c r="F72" t="s">
+        <v>113</v>
+      </c>
+      <c r="G72">
+        <v>336</v>
+      </c>
+      <c r="H72" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>114</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C73">
+        <v>70</v>
+      </c>
+      <c r="D73" t="s">
+        <v>115</v>
+      </c>
+      <c r="E73" t="s">
+        <v>116</v>
+      </c>
+      <c r="F73" t="s">
+        <v>113</v>
+      </c>
+      <c r="G73">
+        <v>341</v>
+      </c>
+      <c r="H73" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>125</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C74">
+        <v>71</v>
+      </c>
+      <c r="D74" t="s">
+        <v>119</v>
+      </c>
+      <c r="E74" t="s">
+        <v>99</v>
+      </c>
+      <c r="F74" t="s">
+        <v>113</v>
+      </c>
+      <c r="G74">
+        <v>345</v>
+      </c>
+      <c r="H74" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -2211,7 +2902,7 @@
           <x14:formula1>
             <xm:f>Types!$A$2:$A$10</xm:f>
           </x14:formula1>
-          <xm:sqref>H1:H1048576</xm:sqref>
+          <xm:sqref>H60:H1048576 H1:H58</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
chore: more monsters raaa
</commit_message>
<xml_diff>
--- a/monsters.xlsx
+++ b/monsters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eterspire Wiki Work\Monster Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF67EE53-273E-4C73-B38B-C2BED11CE51B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8FD012-0E64-4E9D-98F6-7605729B933F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9228" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -508,10 +508,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -828,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F537407C-ED86-44CA-B9EC-6F634CBFD2ED}">
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52:I74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2320,6 +2321,9 @@
       <c r="H52" t="s">
         <v>26</v>
       </c>
+      <c r="I52" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
@@ -2346,6 +2350,9 @@
       <c r="H53" t="s">
         <v>97</v>
       </c>
+      <c r="I53" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
@@ -2372,6 +2379,9 @@
       <c r="H54" t="s">
         <v>20</v>
       </c>
+      <c r="I54" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
@@ -2398,6 +2408,9 @@
       <c r="H55" t="s">
         <v>15</v>
       </c>
+      <c r="I55" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
@@ -2424,6 +2437,9 @@
       <c r="H56" t="s">
         <v>15</v>
       </c>
+      <c r="I56" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
@@ -2450,6 +2466,9 @@
       <c r="H57" t="s">
         <v>52</v>
       </c>
+      <c r="I57" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
@@ -2476,6 +2495,9 @@
       <c r="H58" t="s">
         <v>59</v>
       </c>
+      <c r="I58" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
@@ -2502,6 +2524,9 @@
       <c r="H59" t="s">
         <v>59</v>
       </c>
+      <c r="I59" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
@@ -2528,6 +2553,9 @@
       <c r="H60" t="s">
         <v>20</v>
       </c>
+      <c r="I60" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
@@ -2554,6 +2582,9 @@
       <c r="H61" t="s">
         <v>15</v>
       </c>
+      <c r="I61" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
@@ -2580,6 +2611,9 @@
       <c r="H62" t="s">
         <v>35</v>
       </c>
+      <c r="I62" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
@@ -2606,6 +2640,9 @@
       <c r="H63" t="s">
         <v>52</v>
       </c>
+      <c r="I63" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
@@ -2632,8 +2669,11 @@
       <c r="H64" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I64" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>140</v>
       </c>
@@ -2658,8 +2698,11 @@
       <c r="H65" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I65" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>137</v>
       </c>
@@ -2684,8 +2727,11 @@
       <c r="H66" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I66" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>106</v>
       </c>
@@ -2710,8 +2756,11 @@
       <c r="H67" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I67" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>110</v>
       </c>
@@ -2736,8 +2785,11 @@
       <c r="H68" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I68" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>124</v>
       </c>
@@ -2762,8 +2814,11 @@
       <c r="H69" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I69" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>112</v>
       </c>
@@ -2788,8 +2843,11 @@
       <c r="H70" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I70" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>117</v>
       </c>
@@ -2814,8 +2872,11 @@
       <c r="H71" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I71" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>123</v>
       </c>
@@ -2840,8 +2901,11 @@
       <c r="H72" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I72" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>114</v>
       </c>
@@ -2866,8 +2930,11 @@
       <c r="H73" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I73" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>125</v>
       </c>
@@ -2891,6 +2958,9 @@
       </c>
       <c r="H74" t="s">
         <v>21</v>
+      </c>
+      <c r="I74" s="3">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: more refactors im just making it a chore
</commit_message>
<xml_diff>
--- a/monsters.xlsx
+++ b/monsters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eterspire Wiki Work\Monster Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8FD012-0E64-4E9D-98F6-7605729B933F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBCACC5-25AD-4C2C-BEF4-A9203D5E7669}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9228" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -508,11 +508,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2321,7 +2320,7 @@
       <c r="H52" t="s">
         <v>26</v>
       </c>
-      <c r="I52" s="3">
+      <c r="I52">
         <v>20</v>
       </c>
     </row>
@@ -2350,7 +2349,7 @@
       <c r="H53" t="s">
         <v>97</v>
       </c>
-      <c r="I53" s="3">
+      <c r="I53">
         <v>20</v>
       </c>
     </row>
@@ -2379,7 +2378,7 @@
       <c r="H54" t="s">
         <v>20</v>
       </c>
-      <c r="I54" s="3">
+      <c r="I54">
         <v>20</v>
       </c>
     </row>
@@ -2408,7 +2407,7 @@
       <c r="H55" t="s">
         <v>15</v>
       </c>
-      <c r="I55" s="3">
+      <c r="I55">
         <v>20</v>
       </c>
     </row>
@@ -2437,7 +2436,7 @@
       <c r="H56" t="s">
         <v>15</v>
       </c>
-      <c r="I56" s="3">
+      <c r="I56">
         <v>20</v>
       </c>
     </row>
@@ -2466,7 +2465,7 @@
       <c r="H57" t="s">
         <v>52</v>
       </c>
-      <c r="I57" s="3">
+      <c r="I57">
         <v>20</v>
       </c>
     </row>
@@ -2495,7 +2494,7 @@
       <c r="H58" t="s">
         <v>59</v>
       </c>
-      <c r="I58" s="3">
+      <c r="I58">
         <v>20</v>
       </c>
     </row>
@@ -2524,7 +2523,7 @@
       <c r="H59" t="s">
         <v>59</v>
       </c>
-      <c r="I59" s="3">
+      <c r="I59">
         <v>20</v>
       </c>
     </row>
@@ -2553,7 +2552,7 @@
       <c r="H60" t="s">
         <v>20</v>
       </c>
-      <c r="I60" s="3">
+      <c r="I60">
         <v>20</v>
       </c>
     </row>
@@ -2582,7 +2581,7 @@
       <c r="H61" t="s">
         <v>15</v>
       </c>
-      <c r="I61" s="3">
+      <c r="I61">
         <v>20</v>
       </c>
     </row>
@@ -2611,7 +2610,7 @@
       <c r="H62" t="s">
         <v>35</v>
       </c>
-      <c r="I62" s="3">
+      <c r="I62">
         <v>20</v>
       </c>
     </row>
@@ -2640,7 +2639,7 @@
       <c r="H63" t="s">
         <v>52</v>
       </c>
-      <c r="I63" s="3">
+      <c r="I63">
         <v>20</v>
       </c>
     </row>
@@ -2669,7 +2668,7 @@
       <c r="H64" t="s">
         <v>15</v>
       </c>
-      <c r="I64" s="3">
+      <c r="I64">
         <v>20</v>
       </c>
     </row>
@@ -2698,7 +2697,7 @@
       <c r="H65" t="s">
         <v>15</v>
       </c>
-      <c r="I65" s="3">
+      <c r="I65">
         <v>20</v>
       </c>
     </row>
@@ -2727,7 +2726,7 @@
       <c r="H66" t="s">
         <v>52</v>
       </c>
-      <c r="I66" s="3">
+      <c r="I66">
         <v>20</v>
       </c>
     </row>
@@ -2756,7 +2755,7 @@
       <c r="H67" t="s">
         <v>59</v>
       </c>
-      <c r="I67" s="3">
+      <c r="I67">
         <v>20</v>
       </c>
     </row>
@@ -2785,7 +2784,7 @@
       <c r="H68" t="s">
         <v>59</v>
       </c>
-      <c r="I68" s="3">
+      <c r="I68">
         <v>20</v>
       </c>
     </row>
@@ -2814,7 +2813,7 @@
       <c r="H69" t="s">
         <v>21</v>
       </c>
-      <c r="I69" s="3">
+      <c r="I69">
         <v>20</v>
       </c>
     </row>
@@ -2843,7 +2842,7 @@
       <c r="H70" t="s">
         <v>52</v>
       </c>
-      <c r="I70" s="3">
+      <c r="I70">
         <v>20</v>
       </c>
     </row>
@@ -2872,7 +2871,7 @@
       <c r="H71" t="s">
         <v>15</v>
       </c>
-      <c r="I71" s="3">
+      <c r="I71">
         <v>20</v>
       </c>
     </row>
@@ -2901,7 +2900,7 @@
       <c r="H72" t="s">
         <v>21</v>
       </c>
-      <c r="I72" s="3">
+      <c r="I72">
         <v>20</v>
       </c>
     </row>
@@ -2930,7 +2929,7 @@
       <c r="H73" t="s">
         <v>21</v>
       </c>
-      <c r="I73" s="3">
+      <c r="I73">
         <v>20</v>
       </c>
     </row>
@@ -2959,7 +2958,7 @@
       <c r="H74" t="s">
         <v>21</v>
       </c>
-      <c r="I74" s="3">
+      <c r="I74">
         <v>20</v>
       </c>
     </row>

</xml_diff>